<commit_message>
wrong table in lec0
</commit_message>
<xml_diff>
--- a/highcharts/kenya_cities/cities_table.xlsx
+++ b/highcharts/kenya_cities/cities_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="22940" windowHeight="14860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="22940" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,40 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
@@ -207,7 +240,75 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
@@ -219,119 +320,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom style="medium">
@@ -340,9 +328,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="336">
+  <cellStyleXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -683,22 +695,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="336">
+  <cellStyles count="360">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -867,6 +879,18 @@
     <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1034,6 +1058,18 @@
     <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1363,266 +1399,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H21"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="2.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="31" thickBot="1"/>
-    <row r="2" spans="2:5" ht="31" thickBot="1">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="2:7" ht="31" thickBot="1"/>
+    <row r="2" spans="2:7" ht="31" thickBot="1">
+      <c r="B2" s="15"/>
+      <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="5" t="s">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="16"/>
+      <c r="C3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>76828</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="16"/>
+      <c r="C4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8">
+        <v>139380</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="16"/>
+      <c r="C5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="8">
+        <v>93369</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="16"/>
+      <c r="C6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="8">
+        <v>218557</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="16"/>
+      <c r="C7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F7" s="8">
+        <v>129934</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="16"/>
+      <c r="C8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="8">
+        <v>88869</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="16"/>
+      <c r="C9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8">
+        <v>233231</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="16"/>
+      <c r="C10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>409928</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="16"/>
+      <c r="C11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="8">
+        <v>106187</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="16"/>
+      <c r="C12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8">
+        <v>155896</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="16"/>
+      <c r="C13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="8">
+        <v>104282</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="16"/>
+      <c r="C14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="8">
+        <v>150041</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="16"/>
+      <c r="C15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>107806</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="16"/>
+      <c r="C16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="8">
+        <v>83803</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="16"/>
+      <c r="C17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="8">
+        <v>181966</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="16"/>
+      <c r="C18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="8">
+        <v>307990</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="16"/>
+      <c r="C19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="8">
+        <v>73626</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="16"/>
+      <c r="C20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D20" s="16"/>
+      <c r="E20" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="8">
         <v>238858</v>
       </c>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="5" t="s">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:7" ht="31" thickBot="1">
+      <c r="B21" s="17"/>
+      <c r="C21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="14">
-        <v>233231</v>
-      </c>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="14">
+      <c r="F21" s="9">
         <v>139853</v>
       </c>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="14">
-        <v>129934</v>
-      </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="14">
-        <v>104282</v>
-      </c>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="14">
-        <v>88869</v>
-      </c>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="14">
-        <v>409928</v>
-      </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="14">
-        <v>93369</v>
-      </c>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="14">
-        <v>76828</v>
-      </c>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="14">
-        <v>155896</v>
-      </c>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="14">
-        <v>83803</v>
-      </c>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="14">
-        <v>218557</v>
-      </c>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="14">
-        <v>150041</v>
-      </c>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="14">
-        <v>139380</v>
-      </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="14">
-        <v>307990</v>
-      </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="14">
-        <v>181966</v>
-      </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="14">
-        <v>107806</v>
-      </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="14">
-        <v>106187</v>
-      </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="2:5" ht="31" thickBot="1">
-      <c r="B21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="15">
-        <v>73626</v>
-      </c>
-      <c r="E21" s="12"/>
+      <c r="G21" s="6"/>
     </row>
   </sheetData>
+  <sortState ref="B3:D21">
+    <sortCondition ref="B3:B21"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1637,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1647,17 +1730,17 @@
     <col min="7" max="7" width="11.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7" s="10" customFormat="1">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1669,7 +1752,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="1">
-        <f>SUMIF(A$10:A$28,A2,C$10:C$28)/COUNTIF(A$10:A$28,A2)</f>
+        <f t="shared" ref="C2:C7" si="0">SUMIF(A$10:A$28,A2,C$10:C$28)/COUNTIF(A$10:A$28,A2)</f>
         <v>199254</v>
       </c>
       <c r="E2" t="str">
@@ -1685,11 +1768,11 @@
         <v>24</v>
       </c>
       <c r="C3" s="1">
-        <f>SUMIF(A$10:A$28,A3,C$10:C$28)/COUNTIF(A$10:A$28,A3)</f>
+        <f t="shared" si="0"/>
         <v>193375</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E7" si="0">"{ name: """&amp;A3&amp;""", color: """&amp;B3&amp;"}, "</f>
+        <f t="shared" ref="E3:E7" si="1">"{ name: """&amp;A3&amp;""", color: """&amp;B3&amp;"}, "</f>
         <v xml:space="preserve">{ name: "Kisumu", color: "#d95f02}, </v>
       </c>
     </row>
@@ -1701,11 +1784,11 @@
         <v>25</v>
       </c>
       <c r="C4" s="1">
-        <f>SUMIF(A$10:A$28,A4,C$10:C$28)/COUNTIF(A$10:A$28,A4)</f>
+        <f t="shared" si="0"/>
         <v>169326</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ name: "Machakos", color: "#7570b3}, </v>
       </c>
     </row>
@@ -1717,11 +1800,11 @@
         <v>26</v>
       </c>
       <c r="C5" s="1">
-        <f>SUMIF(A$10:A$28,A5,C$10:C$28)/COUNTIF(A$10:A$28,A5)</f>
+        <f t="shared" si="0"/>
         <v>155837.83333333334</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ name: "Kiambu", color: "#e7298a}, </v>
       </c>
     </row>
@@ -1733,11 +1816,11 @@
         <v>27</v>
       </c>
       <c r="C6" s="1">
-        <f>SUMIF(A$10:A$28,A6,C$10:C$28)/COUNTIF(A$10:A$28,A6)</f>
+        <f t="shared" si="0"/>
         <v>119849.5</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ name: "Kitui", color: "#66a61e}, </v>
       </c>
     </row>
@@ -1749,30 +1832,30 @@
         <v>28</v>
       </c>
       <c r="C7" s="1">
-        <f>SUMIF(A$10:A$28,A7,C$10:C$28)/COUNTIF(A$10:A$28,A7)</f>
+        <f t="shared" si="0"/>
         <v>89906.5</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">{ name: "Trans-Nzoia", color: "#e6ab02}, </v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
@@ -1785,7 +1868,7 @@
         <v>307990</v>
       </c>
       <c r="E10" t="str">
-        <f>"{ name: """&amp;B10&amp;""", color: """&amp;VLOOKUP(A10,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C10&amp;"}, "</f>
+        <f t="shared" ref="E10:E28" si="2">"{ name: """&amp;B10&amp;""", color: """&amp;VLOOKUP(A10,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C10&amp;"}, "</f>
         <v xml:space="preserve">{ name: "Nakuru", color: "#1b9e77", y: 307990}, </v>
       </c>
       <c r="G10"/>
@@ -1801,7 +1884,7 @@
         <v>181966</v>
       </c>
       <c r="E11" t="str">
-        <f>"{ name: """&amp;B11&amp;""", color: """&amp;VLOOKUP(A11,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C11&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Naivasha", color: "#1b9e77", y: 181966}, </v>
       </c>
       <c r="G11"/>
@@ -1817,7 +1900,7 @@
         <v>107806</v>
       </c>
       <c r="E12" t="str">
-        <f>"{ name: """&amp;B12&amp;""", color: """&amp;VLOOKUP(A12,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C12&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Molo", color: "#1b9e77", y: 107806}, </v>
       </c>
       <c r="G12"/>
@@ -1833,7 +1916,7 @@
         <v>409928</v>
       </c>
       <c r="E13" t="str">
-        <f>"{ name: """&amp;B13&amp;""", color: """&amp;VLOOKUP(A13,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C13&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Kisumu", color: "#d95f02", y: 409928}, </v>
       </c>
       <c r="G13"/>
@@ -1849,7 +1932,7 @@
         <v>93369</v>
       </c>
       <c r="E14" t="str">
-        <f>"{ name: """&amp;B14&amp;""", color: """&amp;VLOOKUP(A14,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C14&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Awasi", color: "#d95f02", y: 93369}, </v>
       </c>
       <c r="G14"/>
@@ -1865,7 +1948,7 @@
         <v>76828</v>
       </c>
       <c r="E15" t="str">
-        <f>"{ name: """&amp;B15&amp;""", color: """&amp;VLOOKUP(A15,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C15&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Ahero", color: "#d95f02", y: 76828}, </v>
       </c>
       <c r="G15"/>
@@ -1881,7 +1964,7 @@
         <v>218557</v>
       </c>
       <c r="E16" t="str">
-        <f>"{ name: """&amp;B16&amp;""", color: """&amp;VLOOKUP(A16,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C16&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Kangundo-Tala", color: "#7570b3", y: 218557}, </v>
       </c>
       <c r="G16"/>
@@ -1897,7 +1980,7 @@
         <v>150041</v>
       </c>
       <c r="E17" t="str">
-        <f>"{ name: """&amp;B17&amp;""", color: """&amp;VLOOKUP(A17,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C17&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Machakos", color: "#7570b3", y: 150041}, </v>
       </c>
       <c r="G17"/>
@@ -1913,7 +1996,7 @@
         <v>139380</v>
       </c>
       <c r="E18" t="str">
-        <f>"{ name: """&amp;B18&amp;""", color: """&amp;VLOOKUP(A18,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C18&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Athi River", color: "#7570b3", y: 139380}, </v>
       </c>
       <c r="G18"/>
@@ -1929,7 +2012,7 @@
         <v>238858</v>
       </c>
       <c r="E19" t="str">
-        <f>"{ name: """&amp;B19&amp;""", color: """&amp;VLOOKUP(A19,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C19&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Ruiru", color: "#e7298a", y: 238858}, </v>
       </c>
       <c r="G19"/>
@@ -1945,7 +2028,7 @@
         <v>233231</v>
       </c>
       <c r="E20" t="str">
-        <f>"{ name: """&amp;B20&amp;""", color: """&amp;VLOOKUP(A20,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C20&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Kikuyu", color: "#e7298a", y: 233231}, </v>
       </c>
       <c r="G20"/>
@@ -1961,7 +2044,7 @@
         <v>139853</v>
       </c>
       <c r="E21" t="str">
-        <f>"{ name: """&amp;B21&amp;""", color: """&amp;VLOOKUP(A21,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C21&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Thika", color: "#e7298a", y: 139853}, </v>
       </c>
       <c r="G21"/>
@@ -1977,7 +2060,7 @@
         <v>129934</v>
       </c>
       <c r="E22" t="str">
-        <f>"{ name: """&amp;B22&amp;""", color: """&amp;VLOOKUP(A22,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C22&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Karuri", color: "#e7298a", y: 129934}, </v>
       </c>
       <c r="G22"/>
@@ -1993,7 +2076,7 @@
         <v>104282</v>
       </c>
       <c r="E23" t="str">
-        <f>"{ name: """&amp;B23&amp;""", color: """&amp;VLOOKUP(A23,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C23&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Limuru", color: "#e7298a", y: 104282}, </v>
       </c>
       <c r="G23"/>
@@ -2009,7 +2092,7 @@
         <v>88869</v>
       </c>
       <c r="E24" t="str">
-        <f>"{ name: """&amp;B24&amp;""", color: """&amp;VLOOKUP(A24,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C24&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Kiambu", color: "#e7298a", y: 88869}, </v>
       </c>
       <c r="G24"/>
@@ -2025,7 +2108,7 @@
         <v>155896</v>
       </c>
       <c r="E25" t="str">
-        <f>"{ name: """&amp;B25&amp;""", color: """&amp;VLOOKUP(A25,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C25&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Kitui", color: "#66a61e", y: 155896}, </v>
       </c>
       <c r="G25"/>
@@ -2041,7 +2124,7 @@
         <v>83803</v>
       </c>
       <c r="E26" t="str">
-        <f>"{ name: """&amp;B26&amp;""", color: """&amp;VLOOKUP(A26,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C26&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Mwingi", color: "#66a61e", y: 83803}, </v>
       </c>
       <c r="G26"/>
@@ -2057,7 +2140,7 @@
         <v>106187</v>
       </c>
       <c r="E27" t="str">
-        <f>"{ name: """&amp;B27&amp;""", color: """&amp;VLOOKUP(A27,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C27&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Kitale", color: "#e6ab02", y: 106187}, </v>
       </c>
       <c r="G27"/>
@@ -2073,7 +2156,7 @@
         <v>73626</v>
       </c>
       <c r="E28" t="str">
-        <f>"{ name: """&amp;B28&amp;""", color: """&amp;VLOOKUP(A28,$A$2:$B$7,2,FALSE)&amp;""", y: "&amp;C28&amp;"}, "</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">{ name: "Nandi Hills", color: "#e6ab02", y: 73626}, </v>
       </c>
       <c r="G28"/>

</xml_diff>